<commit_message>
partie de hassen terminé
</commit_message>
<xml_diff>
--- a/courbe.xlsx
+++ b/courbe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasse\Desktop\cours\info\4A\IA\TP\LEFORT\POLYTECH-RESEAUX-DE-NEURONES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasse\Desktop\cours\4A\IA\POLYTECH-RESEAUX-DE-NEURONES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BA21C1-DF94-48CD-A512-157269A7FCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3FDE15-720C-442E-B679-71A86132EDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -6118,19 +6118,19 @@
   <dimension ref="A3:BF21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="J20" sqref="J19:J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.54296875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="19" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="33.5703125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="19" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>6.0101272603236902E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -6308,11 +6308,11 @@
         <v>4.9709583200908698</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
@@ -6422,7 +6422,7 @@
       <c r="BE7" s="3"/>
       <c r="BF7" s="3"/>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -6499,7 +6499,7 @@
         <v>0.67932841892315399</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -6576,7 +6576,7 @@
         <v>1.16313312282497E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -6635,7 +6635,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>1.8521934336465099E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -6753,7 +6753,7 @@
         <v>0.874661928932573</v>
       </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -6812,7 +6812,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>1</v>
       </c>
@@ -6871,7 +6871,7 @@
         <v>2.6874291914291098E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>2</v>
       </c>
@@ -6930,7 +6930,7 @@
         <v>0.95304436277364402</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
@@ -6943,8 +6943,11 @@
       <c r="D19" s="4">
         <v>3</v>
       </c>
+      <c r="E19" s="4">
+        <v>4</v>
+      </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>1</v>
       </c>
@@ -6957,8 +6960,11 @@
       <c r="D20" s="5">
         <v>1.4898156641170401E-2</v>
       </c>
+      <c r="E20" s="5">
+        <v>8.49165538769555E-3</v>
+      </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -6970,6 +6976,9 @@
       </c>
       <c r="D21" s="5">
         <v>0.78550866556966203</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.59740322873909302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>